<commit_message>
updated readme and started adding my steps of what I did. also updated the studen design xlsx file
</commit_message>
<xml_diff>
--- a/student_design.xlsx
+++ b/student_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Artemis\Python\Project\student_feedback_plm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{BA8BF64D-7E98-446D-9E3A-F059E3B68C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5AA1FB-0744-4223-9F10-E291342E2977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14985" yWindow="-19455" windowWidth="29040" windowHeight="18240" xr2:uid="{83258A38-415A-47A7-AA49-054A929294F9}"/>
+    <workbookView xWindow="-20520" yWindow="-19935" windowWidth="29040" windowHeight="18240" xr2:uid="{83258A38-415A-47A7-AA49-054A929294F9}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -36,70 +36,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Design Info</t>
-  </si>
-  <si>
-    <t>Student</t>
-  </si>
-  <si>
-    <t>Matthew</t>
-  </si>
-  <si>
-    <t>Mark</t>
-  </si>
-  <si>
-    <t>Luke</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Overall performance</t>
-  </si>
-  <si>
-    <t>General understanding</t>
-  </si>
-  <si>
-    <t>Contribution level</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>Engagement</t>
   </si>
   <si>
-    <t>Further study level</t>
-  </si>
-  <si>
-    <t>Lab completion</t>
-  </si>
-  <si>
     <t>Punctuality</t>
   </si>
   <si>
-    <t>score of 1 - 4 for the following</t>
-  </si>
-  <si>
-    <t>Key:</t>
-  </si>
-  <si>
-    <t>basic</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>excellent</t>
+    <t>Design Info from brief: https://github.com/chris-reeves1/python29-09-25/blob/main/report/report.MD</t>
+  </si>
+  <si>
+    <t>Student Name</t>
+  </si>
+  <si>
+    <t>Overall Performance</t>
+  </si>
+  <si>
+    <t>General Understanding</t>
+  </si>
+  <si>
+    <t>Contribution Level</t>
+  </si>
+  <si>
+    <t>Lab Completion</t>
+  </si>
+  <si>
+    <t>Further Study Level</t>
+  </si>
+  <si>
+    <t>Scoring Key:</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Okay</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (this is the scoring key that will be used to mark the students)</t>
+  </si>
+  <si>
+    <t>(these are the categories that each student will receive a score for)</t>
+  </si>
+  <si>
+    <t>Score of 1 - 4 for the following categories:</t>
+  </si>
+  <si>
+    <t>Scoring Visual : - This is just an example</t>
+  </si>
+  <si>
+    <t>Student 1</t>
+  </si>
+  <si>
+    <t>Student 2</t>
+  </si>
+  <si>
+    <t>Student 3</t>
+  </si>
+  <si>
+    <t>Student 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +121,37 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -121,10 +161,49 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -133,14 +212,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,119 +581,256 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E7E2B0-F196-4213-8153-21698B149D64}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="22.7109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="12">
+        <v>1</v>
+      </c>
+      <c r="D19" s="12">
+        <v>4</v>
+      </c>
+      <c r="E19" s="12">
+        <v>2</v>
+      </c>
+      <c r="F19" s="12">
+        <v>1</v>
+      </c>
+      <c r="G19" s="12">
+        <v>4</v>
+      </c>
+      <c r="H19" s="12">
+        <v>3</v>
+      </c>
+      <c r="I19" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="12">
+        <v>2</v>
+      </c>
+      <c r="D20" s="12">
+        <v>3</v>
+      </c>
+      <c r="E20" s="12">
+        <v>2</v>
+      </c>
+      <c r="F20" s="12">
+        <v>2</v>
+      </c>
+      <c r="G20" s="12">
+        <v>4</v>
+      </c>
+      <c r="H20" s="12">
+        <v>3</v>
+      </c>
+      <c r="I20" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="12">
+        <v>3</v>
+      </c>
+      <c r="D21" s="12">
+        <v>2</v>
+      </c>
+      <c r="E21" s="12">
+        <v>2</v>
+      </c>
+      <c r="F21" s="13">
+        <v>3</v>
+      </c>
+      <c r="G21" s="12">
+        <v>4</v>
+      </c>
+      <c r="H21" s="12">
+        <v>3</v>
+      </c>
+      <c r="I21" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="12">
+        <v>4</v>
+      </c>
+      <c r="D22" s="12">
+        <v>1</v>
+      </c>
+      <c r="E22" s="13">
+        <v>2</v>
+      </c>
+      <c r="F22" s="12">
+        <v>4</v>
+      </c>
+      <c r="G22" s="12">
+        <v>4</v>
+      </c>
+      <c r="H22" s="12">
+        <v>3</v>
+      </c>
+      <c r="I22" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>3</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added dictinary content etc and testing using print
</commit_message>
<xml_diff>
--- a/student_design.xlsx
+++ b/student_design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Artemis\Python\Project\student_feedback_plm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5AA1FB-0744-4223-9F10-E291342E2977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38D329E-0241-4E96-A6B1-ED7F3CC88194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="-19935" windowWidth="29040" windowHeight="18240" xr2:uid="{83258A38-415A-47A7-AA49-054A929294F9}"/>
+    <workbookView xWindow="-19860" yWindow="-19845" windowWidth="29040" windowHeight="18240" xr2:uid="{83258A38-415A-47A7-AA49-054A929294F9}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -212,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -220,19 +220,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -583,7 +580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E7E2B0-F196-4213-8153-21698B149D64}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -599,50 +598,50 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
+      <c r="B12" s="7"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -650,7 +649,7 @@
       <c r="C17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="6" t="s">
@@ -689,25 +688,25 @@
       <c r="B19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>1</v>
       </c>
-      <c r="D19" s="12">
-        <v>4</v>
-      </c>
-      <c r="E19" s="12">
-        <v>2</v>
-      </c>
-      <c r="F19" s="12">
+      <c r="D19" s="11">
+        <v>4</v>
+      </c>
+      <c r="E19" s="11">
+        <v>2</v>
+      </c>
+      <c r="F19" s="11">
         <v>1</v>
       </c>
-      <c r="G19" s="12">
-        <v>4</v>
-      </c>
-      <c r="H19" s="12">
-        <v>3</v>
-      </c>
-      <c r="I19" s="12">
+      <c r="G19" s="11">
+        <v>4</v>
+      </c>
+      <c r="H19" s="11">
+        <v>3</v>
+      </c>
+      <c r="I19" s="11">
         <v>1</v>
       </c>
     </row>
@@ -715,25 +714,25 @@
       <c r="B20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="12">
-        <v>2</v>
-      </c>
-      <c r="D20" s="12">
-        <v>3</v>
-      </c>
-      <c r="E20" s="12">
-        <v>2</v>
-      </c>
-      <c r="F20" s="12">
-        <v>2</v>
-      </c>
-      <c r="G20" s="12">
-        <v>4</v>
-      </c>
-      <c r="H20" s="12">
-        <v>3</v>
-      </c>
-      <c r="I20" s="12">
+      <c r="C20" s="11">
+        <v>2</v>
+      </c>
+      <c r="D20" s="11">
+        <v>3</v>
+      </c>
+      <c r="E20" s="11">
+        <v>2</v>
+      </c>
+      <c r="F20" s="11">
+        <v>2</v>
+      </c>
+      <c r="G20" s="11">
+        <v>4</v>
+      </c>
+      <c r="H20" s="11">
+        <v>3</v>
+      </c>
+      <c r="I20" s="11">
         <v>2</v>
       </c>
     </row>
@@ -741,25 +740,25 @@
       <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="12">
-        <v>3</v>
-      </c>
-      <c r="D21" s="12">
-        <v>2</v>
-      </c>
-      <c r="E21" s="12">
-        <v>2</v>
-      </c>
-      <c r="F21" s="13">
-        <v>3</v>
-      </c>
-      <c r="G21" s="12">
-        <v>4</v>
-      </c>
-      <c r="H21" s="12">
-        <v>3</v>
-      </c>
-      <c r="I21" s="12">
+      <c r="C21" s="11">
+        <v>3</v>
+      </c>
+      <c r="D21" s="11">
+        <v>2</v>
+      </c>
+      <c r="E21" s="11">
+        <v>2</v>
+      </c>
+      <c r="F21" s="12">
+        <v>3</v>
+      </c>
+      <c r="G21" s="11">
+        <v>4</v>
+      </c>
+      <c r="H21" s="11">
+        <v>3</v>
+      </c>
+      <c r="I21" s="11">
         <v>3</v>
       </c>
     </row>
@@ -767,25 +766,25 @@
       <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="12">
-        <v>4</v>
-      </c>
-      <c r="D22" s="12">
+      <c r="C22" s="11">
+        <v>4</v>
+      </c>
+      <c r="D22" s="11">
         <v>1</v>
       </c>
-      <c r="E22" s="13">
-        <v>2</v>
-      </c>
-      <c r="F22" s="12">
-        <v>4</v>
-      </c>
-      <c r="G22" s="12">
-        <v>4</v>
-      </c>
-      <c r="H22" s="12">
-        <v>3</v>
-      </c>
-      <c r="I22" s="12">
+      <c r="E22" s="12">
+        <v>2</v>
+      </c>
+      <c r="F22" s="11">
+        <v>4</v>
+      </c>
+      <c r="G22" s="11">
+        <v>4</v>
+      </c>
+      <c r="H22" s="11">
+        <v>3</v>
+      </c>
+      <c r="I22" s="11">
         <v>4</v>
       </c>
     </row>
@@ -832,5 +831,6 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>